<commit_message>
schriftliche Aufgabe 3.2 ergaenzt
</commit_message>
<xml_diff>
--- a/Hausaufgabe3/aufgabe31.xlsx
+++ b/Hausaufgabe3/aufgabe31.xlsx
@@ -734,7 +734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -827,18 +829,10 @@
         <v>20</v>
       </c>
       <c r="W1" s="1"/>
-      <c r="X1" s="1">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>25</v>
-      </c>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Hausaufgabe 3 abgabefertig gemacht
</commit_message>
<xml_diff>
--- a/Hausaufgabe3/aufgabe31.xlsx
+++ b/Hausaufgabe3/aufgabe31.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
   <si>
     <t>Prozess</t>
   </si>
@@ -352,19 +352,42 @@
   </si>
   <si>
     <t>terminated</t>
+  </si>
+  <si>
+    <t>Aufgabe 3.1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -379,7 +402,7 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -394,15 +417,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -761,421 +828,467 @@
     <col min="22" max="22" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1">
-        <v>20</v>
-      </c>
+    <row r="1" spans="1:27" ht="15" customHeight="1">
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D7" s="2">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F7" s="2">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H7" s="2">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I7" s="2">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J7" s="2">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K7" s="2">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L7" s="2">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+    </row>
+    <row r="8" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
+    </row>
+    <row r="9" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="E16" s="2">
         <v>14</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="F16" s="2">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="G16" s="2">
         <v>16</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="H16" s="2">
         <v>17</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="I16" s="2">
         <v>18</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="J16" s="2">
         <v>19</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="K16" s="2">
         <v>20</v>
       </c>
-      <c r="U2" s="1" t="s">
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="K17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="H18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="I18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="J18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="K18" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="F19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="H19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="I19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="J19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="K19" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="H20" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="I20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="J20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="K20" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="G21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="H21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="I21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="J21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="K21" s="2" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>